<commit_message>
added userAgent to feedback extraction
</commit_message>
<xml_diff>
--- a/generators/feedback.xlsx
+++ b/generators/feedback.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>userAgent</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>file</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>task_completed</t>
         </is>
@@ -468,10 +473,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-15%E2%80%9314%3A56-Pye6hKXnAGS6JBg?alt=media&amp;token=816f3c38-311b-4b11-b352-ae500ae3c281</t>
         </is>
       </c>
-      <c r="D2" t="b">
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -488,10 +498,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A27-6MLd7kYG1m52LZ2?alt=media&amp;token=dcf2851b-bd3a-4708-921c-7ced54b45c8b</t>
         </is>
       </c>
-      <c r="D3" t="b">
+      <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -508,10 +523,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A34-G1ZxJDi0FnEOsRs?alt=media&amp;token=5ff22268-b8bc-4c53-a4d6-70f4cc790a6c</t>
         </is>
       </c>
-      <c r="D4" t="b">
+      <c r="E4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -528,10 +548,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A37-y5Zskvp9l034AAI?alt=media&amp;token=689aab6a-03d4-47fb-8fcf-c2855d565f14</t>
         </is>
       </c>
-      <c r="D5" t="b">
+      <c r="E5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -548,10 +573,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A39-cYBozINktYPGeA5?alt=media&amp;token=67732728-2cb3-41a2-a6ab-973993927efc</t>
         </is>
       </c>
-      <c r="D6" t="b">
+      <c r="E6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -568,10 +598,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A45-Z5P7DKI7jWVHGXJ?alt=media&amp;token=1126bf84-1f49-4806-837e-93c46dfe3120</t>
         </is>
       </c>
-      <c r="D7" t="b">
+      <c r="E7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -588,10 +623,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A46-0OQC5bbmEm5tPT7?alt=media&amp;token=a3d146fb-df9b-42c8-bf4d-acf4658c1833</t>
         </is>
       </c>
-      <c r="D8" t="b">
+      <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -608,10 +648,15 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A49-gbBrqKoRoU3UJ9F?alt=media&amp;token=1ca914a6-e04c-4a84-8b82-8bdc5ece3b71</t>
         </is>
       </c>
-      <c r="D9" t="b">
+      <c r="E9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -628,10 +673,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A50-9JBC6PHIDIOWI9G?alt=media&amp;token=172dcaf6-f31d-44ad-8957-0371b31e0e5f</t>
         </is>
       </c>
-      <c r="D10" t="b">
+      <c r="E10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -648,10 +698,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A51-BWNeqyluZOGprMA?alt=media&amp;token=741e14a7-4837-40af-ac64-cac84d960ed4</t>
         </is>
       </c>
-      <c r="D11" t="b">
+      <c r="E11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -668,10 +723,15 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A04-5bbEwYFsJGdVsRy?alt=media&amp;token=ad66fe42-8026-422e-814c-b1c8a9d0217c</t>
         </is>
       </c>
-      <c r="D12" t="b">
+      <c r="E12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -688,10 +748,15 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A09-r6jsIU0mE2knwpG?alt=media&amp;token=128e3248-9d6f-4067-98f2-0054c5b08b75</t>
         </is>
       </c>
-      <c r="D13" t="b">
+      <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -708,10 +773,15 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A11-6xrnYBOXxXv4E52?alt=media&amp;token=6fed2eb5-7b54-46f3-b8eb-a2c4c40290b7</t>
         </is>
       </c>
-      <c r="D14" t="b">
+      <c r="E14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -728,10 +798,15 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9312%3A10-b9kX2vhyaBb4tUy?alt=media&amp;token=d00bfb15-9598-4af2-b5bc-46b4c701dd9b</t>
         </is>
       </c>
-      <c r="D15" t="b">
+      <c r="E15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -748,10 +823,15 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A03-nca7uYlebxRLGSq?alt=media&amp;token=ab6bfc97-4187-479d-a151-db95d21bade8</t>
         </is>
       </c>
-      <c r="D16" t="b">
+      <c r="E16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -768,10 +848,15 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A05-m2jVvnqJaBWzExH?alt=media&amp;token=191a95d0-d273-4a56-b692-11f47750f976</t>
         </is>
       </c>
-      <c r="D17" t="b">
+      <c r="E17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -788,10 +873,15 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A09-d8RxYJPmHHe3fEY?alt=media&amp;token=b5fb8490-7974-4f28-b558-71906c4172eb</t>
         </is>
       </c>
-      <c r="D18" t="b">
+      <c r="E18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -808,10 +898,15 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A18-svRrcF9yENTODmW?alt=media&amp;token=60e726cb-561a-4eee-99c2-3aef8e88241a</t>
         </is>
       </c>
-      <c r="D19" t="b">
+      <c r="E19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -828,10 +923,15 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A20-QKk4YXmw2WACdhT?alt=media&amp;token=d948dfff-6449-412d-93aa-191f471ed94a</t>
         </is>
       </c>
-      <c r="D20" t="b">
+      <c r="E20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -848,10 +948,15 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A22-d4heT4gvEwUxSmY?alt=media&amp;token=fe34360e-f9b3-480e-9856-1ecaeccf9fff</t>
         </is>
       </c>
-      <c r="D21" t="b">
+      <c r="E21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -869,10 +974,15 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9313%3A15-scPf1Dlj6G2ffzB?alt=media&amp;token=721078fa-3410-4726-938f-466ed7284016</t>
         </is>
       </c>
-      <c r="D22" t="b">
+      <c r="E22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -889,10 +999,15 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9316%3A41-zeJI7VSaKWiPYiB?alt=media&amp;token=f75c5615-ff7d-4d70-8489-8c4bf0a30059</t>
         </is>
       </c>
-      <c r="D23" t="b">
+      <c r="E23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -909,10 +1024,15 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9318%3A39-9JThZlE8JLsR0JU?alt=media&amp;token=75602d02-3146-44dd-9103-f0404c389a91</t>
         </is>
       </c>
-      <c r="D24" t="b">
+      <c r="E24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -929,10 +1049,15 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9320%3A24-cnE09FKFrs9HskV?alt=media&amp;token=d53b2434-a03a-4864-8b4d-b29531f76b9f</t>
         </is>
       </c>
-      <c r="D25" t="b">
+      <c r="E25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -949,10 +1074,15 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-19%E2%80%9318%3A53-l0neoauIf9h4UkZ?alt=media&amp;token=e028611f-abbc-495d-ac4b-26f5c7d1e970</t>
         </is>
       </c>
-      <c r="D26" t="b">
+      <c r="E26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -969,10 +1099,15 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-19%E2%80%9319%3A11-wABGSBazRdCMzx4?alt=media&amp;token=3b651ec5-c0d3-4551-826c-0a9d1dc0d10a</t>
         </is>
       </c>
-      <c r="D27" t="b">
+      <c r="E27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -989,10 +1124,15 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-20%E2%80%9315%3A59-WAYA0ya6nvA2YP5?alt=media&amp;token=5f3c2355-012b-4571-82b4-d681b647c5bf</t>
         </is>
       </c>
-      <c r="D28" t="b">
+      <c r="E28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1009,10 +1149,15 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-21%E2%80%9318%3A06-DdP7oh0skwTyR9d?alt=media&amp;token=9eebb3e8-6dca-4990-9ba0-61663783a0ec</t>
         </is>
       </c>
-      <c r="D29" t="b">
+      <c r="E29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1029,10 +1174,40 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-21%E2%80%9321%3A21-vQ5fZZEMTJTKHiV?alt=media&amp;token=9a73a531-5ac1-456e-ac86-b3ddc6228f02</t>
         </is>
       </c>
-      <c r="D30" t="b">
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>V01-24-01-08–21:38-2DcdaZD9SXNYol5</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>This is a test feedback</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-24-01-08%E2%80%9321%3A38-2DcdaZD9SXNYol5?alt=media&amp;token=0eb81203-9a3f-4d1f-a13f-d55780e6e087</t>
+        </is>
+      </c>
+      <c r="E31" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added statistics for users
</commit_message>
<xml_diff>
--- a/generators/feedback.xlsx
+++ b/generators/feedback.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,324 +467,302 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>V01-23-12-14–19:26-niX3SZKeGiKP4vw</t>
+          <t>flutter-V04-24-02-18–19:51-qRNDrhXihRBb86N</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Steckt hin und wieder</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2023-12-15T14:56:56.597</t>
-        </is>
+          <t>Level 9 hat ohne einen möglichen Zug gestartet. es kam gleich die Fehlermeldung, dass kein Zug möglich ist, usw...</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>45341.9790859838</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-15%E2%80%9314%3A56-Pye6hKXnAGS6JBg?alt=media&amp;token=816f3c38-311b-4b11-b352-ae500ae3c281</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9323%3A29-mTEMsWKYtwoCAPb?alt=media&amp;token=fa6482ed-37a2-4463-ac91-c942a1576d89</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>level 3 eben abgestürzt und rückkehr zu startscreen</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:27:06.563</t>
-        </is>
+          <t>4 feedback</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45341.53525732639</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A27-6MLd7kYG1m52LZ2?alt=media&amp;token=dcf2851b-bd3a-4708-921c-7ced54b45c8b</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A50-HYlUWTP0c7AQixB?alt=media&amp;token=a839b713-c2e5-44c0-bf94-de507371ca90</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>innerhalb des Spiels "Du"-Form</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:35:01.622</t>
-        </is>
+          <t>3 feedback</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45341.53482371528</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A34-G1ZxJDi0FnEOsRs?alt=media&amp;token=5ff22268-b8bc-4c53-a4d6-70f4cc790a6c</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A50-M2chbwGfLbe9eAF?alt=media&amp;token=ab1d9c98-b4fa-4a00-98f5-84dc42e4bf1e</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(nochmalige) info über die funktion der booster wäre an dieser stelle hilfreich</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:37:15.480</t>
-        </is>
+          <t>second feedback</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45341.53437194444</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A37-y5Zskvp9l034AAI?alt=media&amp;token=689aab6a-03d4-47fb-8fcf-c2855d565f14</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A49-TZqOyHwDwfDP0S1?alt=media&amp;token=e6528c6a-7ca0-4d0b-ad98-b871b6f33df7</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>info oder einsatztipp über den booster wäre hilfreich, ich weiß jetzt nicht (mehr) was damit zu tun ist.</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:39:09.859</t>
-        </is>
+          <t xml:space="preserve">nochmal ein test feedback </t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45341.50729023148</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A39-cYBozINktYPGeA5?alt=media&amp;token=67732728-2cb3-41a2-a6ab-973993927efc</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A10-bqbfZjkA52vniVJ?alt=media&amp;token=e6e35670-c037-4240-a2c4-acb28d96a1aa</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-18–17:59-c4MaSoluDqTLqxP</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">kann man da  an dieser stelle irgendwie hinweis geben, dass da unten der counter ist? </t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:45:06.098</t>
-        </is>
+          <t>bei den instruktionen ist hier eine zeile platz mitten im text</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45340.757124375</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 13; SAMSUNG SM-G781B) AppleWebKit/537.36 (KHTML, like Gecko) SamsungBrowser/23.0 Chrome/115.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A45-Z5P7DKI7jWVHGXJ?alt=media&amp;token=1126bf84-1f49-4806-837e-93c46dfe3120</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9318%3A10-hAKKqjcmPEqUdF9?alt=media&amp;token=388454c1-615d-4e5c-985b-b75f6311a6f4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-18–17:00-1yCnLXN9Mo3ar27</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>irgendwie fehlt audio also hintergrundmusik, geräusche bei erfolg, verlieren etc</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:46:49.290</t>
-        </is>
+          <t xml:space="preserve">siehe Foto; Züge aus obwohl noch genug da waren </t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45340.71798287037</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A46-0OQC5bbmEm5tPT7?alt=media&amp;token=a3d146fb-df9b-42c8-bf4d-acf4658c1833</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9317%3A13-SpIytlCIPTKNmJK?alt=media&amp;token=644759b1-797c-4624-a1c1-0700343576b1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-18–17:00-1yCnLXN9Mo3ar27</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>glaube eben gewonnen zu haben obwohl nur 2200 von 2800 pkt geschafft</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:49:44.410</t>
-        </is>
+          <t>Handy wird schnell warm und beim Feedback schreiben ist's sehr laggy 
+ansonsten cute :)</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45340.7135746875</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A49-gbBrqKoRoU3UJ9F?alt=media&amp;token=1ca914a6-e04c-4a84-8b82-8bdc5ece3b71</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9317%3A07-R4lduUDjzkW1SbJ?alt=media&amp;token=244ab44d-157b-4fbb-bf80-8c12912d74e7</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>flutter-V04-24-02-18–17:00-1yCnLXN9Mo3ar27</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>was mache ich da mit dem grün gestreiften?</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:50:25.835</t>
-        </is>
+          <t>Handy wird schnell warm und beim Feedback schreiben ist's sehr laggy 
+ansonsten cute :)</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45340.71344337963</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A50-9JBC6PHIDIOWI9G?alt=media&amp;token=172dcaf6-f31d-44ad-8957-0371b31e0e5f</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9317%3A07-eggGWG3Fy7wZcXL?alt=media&amp;token=05e696f3-a2c4-4350-9dcb-f804ee15e8ae</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>testVersion-V03-24-02-06–18:30-ybL4tMRFHX7cA4O</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>tw kann mann jellies nur schwer verschieben bzw auch nur in ein richtung</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2023-12-16T18:51:18.048</t>
-        </is>
+          <t>lol</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45328.77146932871</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A51-BWNeqyluZOGprMA?alt=media&amp;token=741e14a7-4837-40af-ac64-cac84d960ed4</t>
+          <t>nothing do download</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-11–17:51-JAGk9gyXqpsRFMK</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>wollte eben Level 7 starten und davor den gestreiften um 100$ erworben. aber Rückkehr zum startscreen</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2023-12-16T19:04:50.162</t>
-        </is>
+          <t>This is a test feedback</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45299.90180064815</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A04-5bbEwYFsJGdVsRy?alt=media&amp;token=ad66fe42-8026-422e-814c-b1c8a9d0217c</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-24-01-08%E2%80%9321%3A38-2DcdaZD9SXNYol5?alt=media&amp;token=0eb81203-9a3f-4d1f-a13f-d55780e6e087</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>irgendwas will der grüne gestreifte schwankende da unten mitteilen aber nur was? lenkt irgendwie ab weil Funktion hat er da doch keine oder wenn ja welche?</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2023-12-16T19:09:34.228</t>
-        </is>
+          <t xml:space="preserve">die Push-Benachrichtigungen könnten häufiger erfolgen um die Leute im Spiel zu behalten. bislang erfolgte innerhalb von 4 Tagen nur eine Benachrichtigung. </t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45281.89000127315</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A09-r6jsIU0mE2knwpG?alt=media&amp;token=128e3248-9d6f-4067-98f2-0054c5b08b75</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-21%E2%80%9321%3A21-vQ5fZZEMTJTKHiV?alt=media&amp;token=9a73a531-5ac1-456e-ac86-b3ddc6228f02</t>
         </is>
       </c>
     </row>
@@ -792,13 +774,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Darstellungsproblem?</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2023-12-16T19:11:32.724</t>
-        </is>
+          <t>was mache ich mit den XP?</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45281.75451850695</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -807,52 +787,48 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A11-6xrnYBOXxXv4E52?alt=media&amp;token=6fed2eb5-7b54-46f3-b8eb-a2c4c40290b7</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-21%E2%80%9318%3A06-DdP7oh0skwTyR9d?alt=media&amp;token=9eebb3e8-6dca-4990-9ba0-61663783a0ec</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>möchte den grünen Jelly nach links verschieben, geht nicht. sehr wohl aber der blauer nach rechts... einige Male beobachtet, auch vertikal...</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2023-12-17T12:10:21.470</t>
-        </is>
+          <t>bei manchen Leveln ist das Ziel bereits mit ein- oder zwei Spielzügen erreicht. ist das Absicht?</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45280.6665641088</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9312%3A10-b9kX2vhyaBb4tUy?alt=media&amp;token=d00bfb15-9598-4af2-b5bc-46b4c701dd9b</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-20%E2%80%9315%3A59-WAYA0ya6nvA2YP5?alt=media&amp;token=5f3c2355-012b-4571-82b4-d681b647c5bf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>das ist die version ohne jegliches pattern, warum dann pushinfos? kommen die trotzdem?</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2023-12-17T18:03:46.756</t>
-        </is>
+          <t>bei der Anzeige des high Scores werden andere Spieler mit username angezeigt, obwohl bei Spielbeginn gar kein username ausgewählt werden kann. gibt es dazu noch eine Lösung?</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45279.79937474537</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -861,296 +837,274 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A03-nca7uYlebxRLGSq?alt=media&amp;token=ab6bfc97-4187-479d-a151-db95d21bade8</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-19%E2%80%9319%3A11-wABGSBazRdCMzx4?alt=media&amp;token=3b651ec5-c0d3-4551-826c-0a9d1dc0d10a</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>pushinfo zur täglichen Belohnung wäre ev spannend? die tägliche Belohnung eben mehr zufällig entdeckt</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>2023-12-17T18:05:55.674</t>
-        </is>
+          <t>leider stürzt jedes zweite Level beim Laden ab. danach kommt man wieder auf den Bildschirm zur levelauswahl und muss wieder zum richtigen Level hinunterscrollen</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45279.78736309028</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A05-m2jVvnqJaBWzExH?alt=media&amp;token=191a95d0-d273-4a56-b692-11f47750f976</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-19%E2%80%9318%3A53-l0neoauIf9h4UkZ?alt=media&amp;token=e028611f-abbc-495d-ac4b-26f5c7d1e970</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-18–20:21-sXeMKhpCmBR9eA2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>tägliche Belohnung bitte aus dem burgermenü raus und irgendwie einladend und optisch hervorgehoben auf die spieloberfläche legen. sonst schaut da denke ich niemand nach. zusätzlich ev auch mit Push bewerben.</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2023-12-17T18:09:15.122</t>
-        </is>
+          <t>jellies lassen sich fast nie tauschen</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45278.85038525463</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A09-d8RxYJPmHHe3fEY?alt=media&amp;token=b5fb8490-7974-4f28-b558-71906c4172eb</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9320%3A24-cnE09FKFrs9HskV?alt=media&amp;token=d53b2434-a03a-4864-8b4d-b29531f76b9f</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>in der Erklärung werden sonderjellies erklärt aber auch booster erwähnt und bei der kaufmöglichkeit heißen dann alle booster?!</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2023-12-17T18:18:30.282</t>
-        </is>
+          <t>iOS 17.2: bei spiel 8, ist das Spiel mehrfach geschlossen worden und ich bin zur levelauswahl zurückgekommen.</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45278.77733798611</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A18-svRrcF9yENTODmW?alt=media&amp;token=60e726cb-561a-4eee-99c2-3aef8e88241a</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9318%3A39-9JThZlE8JLsR0JU?alt=media&amp;token=75602d02-3146-44dd-9103-f0404c389a91</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>bitte passende Musik und Geräusche einbauen. Ausschaltung muss möglich sein</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2023-12-17T18:20:06.228</t>
-        </is>
+          <t>Nutzung auf iOS 16.7.2: leider lassen sich die jellys nicht richtig bewegen. es wirkt als würde das Spiel nicht auf die wischbewegunh reagieren. hilfreich wäre auch, wenn sich der angetippte jelly mitbewegt</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45278.69559321759</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A20-QKk4YXmw2WACdhT?alt=media&amp;token=d948dfff-6449-412d-93aa-191f471ed94a</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9316%3A41-zeJI7VSaKWiPYiB?alt=media&amp;token=f75c5615-ff7d-4d70-8489-8c4bf0a30059</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>das ist die version ohne jegliches pattern, warum dann pushinfos? kommen die trotzdem?</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>2023-12-17T18:22:47.615</t>
-        </is>
+          <t xml:space="preserve">Text passt nicht mit den abgebildeten Dingen zusammen. Highscoretafel (3) ist der Dollarcounter und Anzahl der Münzen (4) ist das Burgermenü... bitte alle Texte prüfen und möglichst vereinfachen. Auch wäre eine Info direkt auf der Spielfläche zumindest beim ersten Spiel hilfreich. Ins Burgermenü schaut denke ich kaum jemand wegen Anleitung oder Tagesbelohnung etc
+kann leider keine Bilder mehr in der Feedbackfunktion anhängen, weiß nicht warum </t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45278.5523871412</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A22-d4heT4gvEwUxSmY?alt=media&amp;token=fe34360e-f9b3-480e-9856-1ecaeccf9fff</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9313%3A15-scPf1Dlj6G2ffzB?alt=media&amp;token=721078fa-3410-4726-938f-466ed7284016</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Text passt nicht mit den abgebildeten Dingen zusammen. Highscoretafel (3) ist der Dollarcounter und Anzahl der Münzen (4) ist das Burgermenü... bitte alle Texte prüfen und möglichst vereinfachen. Auch wäre eine Info direkt auf der Spielfläche zumindest beim ersten Spiel hilfreich. Ins Burgermenü schaut denke ich kaum jemand wegen Anleitung oder Tagesbelohnung etc
-kann leider keine Bilder mehr in der Feedbackfunktion anhängen, weiß nicht warum </t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2023-12-18T13:15:26.249</t>
-        </is>
+          <t>das ist die version ohne jegliches pattern, warum dann pushinfos? kommen die trotzdem?</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45277.76582887732</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9313%3A15-scPf1Dlj6G2ffzB?alt=media&amp;token=721078fa-3410-4726-938f-466ed7284016</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A22-d4heT4gvEwUxSmY?alt=media&amp;token=fe34360e-f9b3-480e-9856-1ecaeccf9fff</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nutzung auf iOS 16.7.2: leider lassen sich die jellys nicht richtig bewegen. es wirkt als würde das Spiel nicht auf die wischbewegunh reagieren. hilfreich wäre auch, wenn sich der angetippte jelly mitbewegt</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>2023-12-18T16:41:39.254</t>
-        </is>
+          <t>bitte passende Musik und Geräusche einbauen. Ausschaltung muss möglich sein</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45277.76396097222</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_7_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9316%3A41-zeJI7VSaKWiPYiB?alt=media&amp;token=f75c5615-ff7d-4d70-8489-8c4bf0a30059</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A20-QKk4YXmw2WACdhT?alt=media&amp;token=d948dfff-6449-412d-93aa-191f471ed94a</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>iOS 17.2: bei spiel 8, ist das Spiel mehrfach geschlossen worden und ich bin zur levelauswahl zurückgekommen.</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>2023-12-18T18:39:22.002</t>
-        </is>
+          <t>in der Erklärung werden sonderjellies erklärt aber auch booster erwähnt und bei der kaufmöglichkeit heißen dann alle booster?!</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45277.76285048611</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9318%3A39-9JThZlE8JLsR0JU?alt=media&amp;token=75602d02-3146-44dd-9103-f0404c389a91</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A18-svRrcF9yENTODmW?alt=media&amp;token=60e726cb-561a-4eee-99c2-3aef8e88241a</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>V01-23-12-18–20:21-sXeMKhpCmBR9eA2</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>jellies lassen sich fast nie tauschen</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>2023-12-18T20:24:33.286</t>
-        </is>
+          <t>tägliche Belohnung bitte aus dem burgermenü raus und irgendwie einladend und optisch hervorgehoben auf die spieloberfläche legen. sonst schaut da denke ich niemand nach. zusätzlich ev auch mit Push bewerben.</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>45277.75642502315</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-18%E2%80%9320%3A24-cnE09FKFrs9HskV?alt=media&amp;token=d53b2434-a03a-4864-8b4d-b29531f76b9f</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A09-d8RxYJPmHHe3fEY?alt=media&amp;token=b5fb8490-7974-4f28-b558-71906c4172eb</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>leider stürzt jedes zweite Level beim Laden ab. danach kommt man wieder auf den Bildschirm zur levelauswahl und muss wieder zum richtigen Level hinunterscrollen</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>2023-12-19T18:53:48.171</t>
-        </is>
+          <t>pushinfo zur täglichen Belohnung wäre ev spannend? die tägliche Belohnung eben mehr zufällig entdeckt</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>45277.75411659722</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-19%E2%80%9318%3A53-l0neoauIf9h4UkZ?alt=media&amp;token=e028611f-abbc-495d-ac4b-26f5c7d1e970</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A05-m2jVvnqJaBWzExH?alt=media&amp;token=191a95d0-d273-4a56-b692-11f47750f976</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>bei der Anzeige des high Scores werden andere Spieler mit username angezeigt, obwohl bei Spielbeginn gar kein username ausgewählt werden kann. gibt es dazu noch eine Lösung?</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>2023-12-19T19:11:05.978</t>
-        </is>
+          <t>das ist die version ohne jegliches pattern, warum dann pushinfos? kommen die trotzdem?</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>45277.75262449074</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1159,34 +1113,32 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-19%E2%80%9319%3A11-wABGSBazRdCMzx4?alt=media&amp;token=3b651ec5-c0d3-4551-826c-0a9d1dc0d10a</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9318%3A03-nca7uYlebxRLGSq?alt=media&amp;token=ab6bfc97-4187-479d-a151-db95d21bade8</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>bei manchen Leveln ist das Ziel bereits mit ein- oder zwei Spielzügen erreicht. ist das Absicht?</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>2023-12-20T15:59:51.139</t>
-        </is>
+          <t>möchte den grünen Jelly nach links verschieben, geht nicht. sehr wohl aber der blauer nach rechts... einige Male beobachtet, auch vertikal...</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>45277.50719293982</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-20%E2%80%9315%3A59-WAYA0ya6nvA2YP5?alt=media&amp;token=5f3c2355-012b-4571-82b4-d681b647c5bf</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-17%E2%80%9312%3A10-b9kX2vhyaBb4tUy?alt=media&amp;token=d00bfb15-9598-4af2-b5bc-46b4c701dd9b</t>
         </is>
       </c>
     </row>
@@ -1198,13 +1150,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>was mache ich mit den XP?</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>2023-12-21T18:06:30.399</t>
-        </is>
+          <t>Darstellungsproblem?</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>45276.79968430556</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1213,306 +1163,307 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-21%E2%80%9318%3A06-DdP7oh0skwTyR9d?alt=media&amp;token=9eebb3e8-6dca-4990-9ba0-61663783a0ec</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A11-6xrnYBOXxXv4E52?alt=media&amp;token=6fed2eb5-7b54-46f3-b8eb-a2c4c40290b7</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>V01-23-12-18–16:31-EEgROYdoZgbbyRF</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">die Push-Benachrichtigungen könnten häufiger erfolgen um die Leute im Spiel zu behalten. bislang erfolgte innerhalb von 4 Tagen nur eine Benachrichtigung. </t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>2023-12-21T21:21:36.110</t>
-        </is>
+          <t>irgendwas will der grüne gestreifte schwankende da unten mitteilen aber nur was? lenkt irgendwie ab weil Funktion hat er da doch keine oder wenn ja welche?</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>45276.79831282407</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-21%E2%80%9321%3A21-vQ5fZZEMTJTKHiV?alt=media&amp;token=9a73a531-5ac1-456e-ac86-b3ddc6228f02</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A09-r6jsIU0mE2knwpG?alt=media&amp;token=128e3248-9d6f-4067-98f2-0054c5b08b75</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>V01-23-12-11–17:51-JAGk9gyXqpsRFMK</t>
+          <t>V01-23-12-11–18:55-fISzQVlhdN1kyS7</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>This is a test feedback</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>2024-01-08T21:38:35.576</t>
-        </is>
+          <t>wollte eben Level 7 starten und davor den gestreiften um 100$ erworben. aber Rückkehr zum startscreen</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>45276.79502502315</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/120.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_5 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.5 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-24-01-08%E2%80%9321%3A38-2DcdaZD9SXNYol5?alt=media&amp;token=0eb81203-9a3f-4d1f-a13f-d55780e6e087</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9319%3A04-5bbEwYFsJGdVsRy?alt=media&amp;token=ad66fe42-8026-422e-814c-b1c8a9d0217c</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-18–17:00-1yCnLXN9Mo3ar27</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Handy wird schnell warm und beim Feedback schreiben ist's sehr laggy 
-ansonsten cute :)</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>2024-02-18T17:07:32.853</t>
-        </is>
+          <t>tw kann mann jellies nur schwer verschieben bzw auch nur in ein richtung</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>45276.78562555555</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9317%3A07-R4lduUDjzkW1SbJ?alt=media&amp;token=244ab44d-157b-4fbb-bf80-8c12912d74e7</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A51-BWNeqyluZOGprMA?alt=media&amp;token=741e14a7-4837-40af-ac64-cac84d960ed4</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-18–17:00-1yCnLXN9Mo3ar27</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Handy wird schnell warm und beim Feedback schreiben ist's sehr laggy 
-ansonsten cute :)</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>2024-02-18T17:07:21.508</t>
-        </is>
+          <t>was mache ich da mit dem grün gestreiften?</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45276.78502123843</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9317%3A07-eggGWG3Fy7wZcXL?alt=media&amp;token=05e696f3-a2c4-4350-9dcb-f804ee15e8ae</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A50-9JBC6PHIDIOWI9G?alt=media&amp;token=172dcaf6-f31d-44ad-8957-0371b31e0e5f</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-18–17:00-1yCnLXN9Mo3ar27</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">siehe Foto; Züge aus obwohl noch genug da waren </t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>2024-02-18T17:13:53.720</t>
-        </is>
+          <t>glaube eben gewonnen zu haben obwohl nur 2200 von 2800 pkt geschafft</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>45276.78454178241</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_3_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.3.1 Mobile/15E148 Safari/604.1</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9317%3A13-SpIytlCIPTKNmJK?alt=media&amp;token=644759b1-797c-4624-a1c1-0700343576b1</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A49-gbBrqKoRoU3UJ9F?alt=media&amp;token=1ca914a6-e04c-4a84-8b82-8bdc5ece3b71</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-18–17:59-c4MaSoluDqTLqxP</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>bei den instruktionen ist hier eine zeile platz mitten im text</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>2024-02-18T18:10:15.546</t>
-        </is>
+          <t>irgendwie fehlt audio also hintergrundmusik, geräusche bei erfolg, verlieren etc</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>45276.78251493056</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 13; SAMSUNG SM-G781B) AppleWebKit/537.36 (KHTML, like Gecko) SamsungBrowser/23.0 Chrome/115.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-18%E2%80%9318%3A10-hAKKqjcmPEqUdF9?alt=media&amp;token=388454c1-615d-4e5c-985b-b75f6311a6f4</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A46-0OQC5bbmEm5tPT7?alt=media&amp;token=a3d146fb-df9b-42c8-bf4d-acf4658c1833</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">nochmal ein test feedback </t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>2024-02-19T12:10:29.876</t>
-        </is>
+          <t xml:space="preserve">kann man da  an dieser stelle irgendwie hinweis geben, dass da unten der counter ist? </t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>45276.7813205787</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A10-bqbfZjkA52vniVJ?alt=media&amp;token=e6e35670-c037-4240-a2c4-acb28d96a1aa</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A45-Z5P7DKI7jWVHGXJ?alt=media&amp;token=1126bf84-1f49-4806-837e-93c46dfe3120</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>second feedback</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>2024-02-19T12:49:29.736</t>
-        </is>
+          <t>info oder einsatztipp über den booster wäre hilfreich, ich weiß jetzt nicht (mehr) was damit zu tun ist.</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>45276.77719744213</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A49-TZqOyHwDwfDP0S1?alt=media&amp;token=e6528c6a-7ca0-4d0b-ad98-b871b6f33df7</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A39-cYBozINktYPGeA5?alt=media&amp;token=67732728-2cb3-41a2-a6ab-973993927efc</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4 feedback</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>2024-02-19T12:50:46.233</t>
-        </is>
+          <t>(nochmalige) info über die funktion der booster wäre an dieser stelle hilfreich</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>45276.77587361111</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A50-HYlUWTP0c7AQixB?alt=media&amp;token=a839b713-c2e5-44c0-bf94-de507371ca90</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A37-y5Zskvp9l034AAI?alt=media&amp;token=689aab6a-03d4-47fb-8fcf-c2855d565f14</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>flutter-V04-24-02-16–13:59-cqub4DQlfSwoHIZ</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3 feedback</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>2024-02-19T12:50:08.769</t>
-        </is>
+          <t>innerhalb des Spiels "Du"-Form</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>45276.7743243287</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Linux; Android 10; K) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Mobile Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2Fflutter-V04-24-02-19%E2%80%9312%3A50-M2chbwGfLbe9eAF?alt=media&amp;token=ab1d9c98-b4fa-4a00-98f5-84dc42e4bf1e</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A34-G1ZxJDi0FnEOsRs?alt=media&amp;token=5ff22268-b8bc-4c53-a4d6-70f4cc790a6c</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>testVersion-V03-24-02-06–18:30-ybL4tMRFHX7cA4O</t>
+          <t>V01-23-12-13–16:00-IR9Ncrq1ALXXwCb</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>lol</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>2024-02-06T18:30:54.950</t>
-        </is>
+          <t>level 3 eben abgestürzt und rückkehr zu startscreen</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>45276.76882596065</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/121.0.0.0 Safari/537.36</t>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_2 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.2 Mobile/15E148 Safari/604.1</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>nothing do download</t>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-16%E2%80%9318%3A27-6MLd7kYG1m52LZ2?alt=media&amp;token=dcf2851b-bd3a-4708-921c-7ced54b45c8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>V01-23-12-14–19:26-niX3SZKeGiKP4vw</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Steckt hin und wieder</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>45275.62287728009</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 16_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://firebasestorage.googleapis.com/v0/b/darkpatterns-ac762.appspot.com/o/feedback%2FV01-23-12-15%E2%80%9314%3A56-Pye6hKXnAGS6JBg?alt=media&amp;token=816f3c38-311b-4b11-b352-ae500ae3c281</t>
         </is>
       </c>
     </row>

</xml_diff>